<commit_message>
começando a add no banco de dados  em excel
</commit_message>
<xml_diff>
--- a/banco_de_dados.xlsx
+++ b/banco_de_dados.xlsx
@@ -1,43 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\Programação\Requisicao_combustivel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9247B50E-064D-40F2-A6F7-E4F1E82E9671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Solicitante</t>
+  </si>
+  <si>
+    <t>Motorista</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Preço Unitário</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Observação</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Teste para buscar valores</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,95 +98,63 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4045D39F-DAAE-4D1E-898F-46F555374D61}" name="Tabela1" displayName="Tabela1" ref="A1:I1048575" totalsRowShown="0">
+  <autoFilter ref="A1:I1048575" xr:uid="{4045D39F-DAAE-4D1E-898F-46F555374D61}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{B33E8AC3-E4D9-4ADB-8C9E-8C40A9EFEF9D}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{36953C48-3AA3-41A3-A9E1-18A03307CC63}" name="Solicitante"/>
+    <tableColumn id="3" xr3:uid="{88FE399E-12E9-4BB2-9652-02D28B1112E1}" name="Motorista"/>
+    <tableColumn id="4" xr3:uid="{4FCA8CEA-37E6-4D2D-A968-7F9A9B39DC92}" name="Categoria"/>
+    <tableColumn id="5" xr3:uid="{271E1342-245D-4A7C-A676-038F9ABD2A1C}" name="Quantidade" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7E778FC5-3CEE-4039-82E3-55100CE1D18D}" name="Preço Unitário" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{C91F1FAB-9021-49E1-8A6C-769C1DD45341}" name="Total" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{1DC86F93-3CCC-4143-8A78-37E16CEAD85A}" name="Data"/>
+    <tableColumn id="9" xr3:uid="{DA6D3514-D8A7-49F2-A3BF-78289D6BAE2C}" name="Observação"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,42 +441,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A147A2BC-FDAA-470C-AF36-21FEF20BDD66}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>um</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>dois</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>três</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>cinco</t>
-        </is>
-      </c>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44888</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
att req in progress
feito até a parte de buscar dados, falta o save e o imprimir
</commit_message>
<xml_diff>
--- a/banco_de_dados.xlsx
+++ b/banco_de_dados.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1116,10 +1116,8 @@
       <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="A21" t="n">
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1147,6 +1145,109 @@
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Adilson</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Adilson</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Filtro de óleo</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>30/11/2022</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Adilson</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Adilson</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Etanol</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>9</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>30/11/2022</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Gabriel</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Adilson</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Filtro de óleo</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>30/11/2022</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
base para o pdf
</commit_message>
<xml_diff>
--- a/banco_de_dados.xlsx
+++ b/banco_de_dados.xlsx
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F2" t="n">
         <v>10</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -534,14 +534,18 @@
           <t>Filtro de óleo</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>200</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -573,12 +577,10 @@
           <t>Gasolina</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>0</v>
       </c>
@@ -608,14 +610,12 @@
           <t>Gasolina</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>30</v>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>10</v>
       </c>
       <c r="G5" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>

</xml_diff>